<commit_message>
added new dataset for lec 4
</commit_message>
<xml_diff>
--- a/Code/car_maintenance.xlsx
+++ b/Code/car_maintenance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="19">
   <si>
     <t>PART_1023</t>
   </si>
@@ -37,9 +37,6 @@
     <t>acc</t>
   </si>
   <si>
-    <t>failure</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
@@ -52,10 +49,28 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>0.7</t>
-  </si>
-  <si>
     <t>0.05</t>
+  </si>
+  <si>
+    <t>FOLLOW-UP</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>PART_02</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>unacc</t>
   </si>
 </sst>
 </file>
@@ -397,19 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,153 +433,640 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
+      <c r="F32" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>